<commit_message>
added FLL Scoring and integration with challonge
</commit_message>
<xml_diff>
--- a/public/uploads/robobowl_scoresheet_acadia.xlsx
+++ b/public/uploads/robobowl_scoresheet_acadia.xlsx
@@ -152,7 +152,7 @@
     <numFmt numFmtId="168" formatCode="0.00000"/>
     <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -214,6 +214,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -227,12 +234,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FFFCD5B5"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -249,7 +262,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFCD5B5"/>
-        <bgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
     <fill>
@@ -259,12 +272,38 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="31">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF4F81BD"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF4F81BD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -490,7 +529,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -514,11 +553,17 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -527,11 +572,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -539,7 +584,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -547,54 +592,46 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -607,39 +644,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="10" fillId="2" borderId="17" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="10" fillId="2" borderId="18" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="10" fillId="2" borderId="19" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="5" borderId="16" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="18" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="11" fillId="3" borderId="19" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="3" borderId="20" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="3" borderId="21" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -647,79 +688,89 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="4" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="10" fillId="2" borderId="26" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="10" fillId="2" borderId="27" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="5" borderId="25" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="3" borderId="28" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="27" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="3" borderId="29" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Total" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Input" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Output" xfId="22" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -738,10 +789,10 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF7F7F7F"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFCD5B5"/>
       <rgbColor rgb="FFDBEEF4"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -762,7 +813,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFCD5B5"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -777,7 +828,7 @@
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF3F3F76"/>
       <rgbColor rgb="FF3F3F3F"/>
     </indexedColors>
   </colors>
@@ -789,10 +840,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A15:O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -920,41 +971,33 @@
       <c r="B5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="22" t="n">
-        <v>20</v>
-      </c>
-      <c r="D5" s="23" t="n">
-        <v>65</v>
-      </c>
-      <c r="E5" s="24" t="n">
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="24" t="str">
         <f aca="false">IF(ISBLANK(D5),"no data",ABS($F$2-D5)/$F$2)</f>
-        <v>0.31578947368421</v>
+        <v>no data</v>
       </c>
       <c r="F5" s="25" t="n">
         <f aca="false">IF(ISBLANK(D5),C5,IF(E5&gt;1,C5,C5+11*(1-E5)))</f>
-        <v>27.5263157894737</v>
-      </c>
-      <c r="G5" s="26" t="n">
-        <v>30</v>
-      </c>
-      <c r="H5" s="27" t="n">
-        <v>200</v>
-      </c>
-      <c r="I5" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="26"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="24" t="str">
         <f aca="false">IF(ISBLANK(H5),"no data",ABS($J$2-H5)/$J$2)</f>
-        <v>0.134199134199134</v>
+        <v>no data</v>
       </c>
       <c r="J5" s="28" t="n">
         <f aca="false">IF(ISBLANK(H5),G5,IF(I5&gt;1,G5-17,G5+11*(1-I5)))</f>
-        <v>39.5238095238095</v>
+        <v>0</v>
       </c>
       <c r="K5" s="29" t="n">
         <f aca="false">AVERAGE(F5,J5)</f>
-        <v>33.5250626566416</v>
+        <v>0</v>
       </c>
       <c r="L5" s="30" t="n">
         <f aca="false">RANK(K5, $K$5:$K$14)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M5" s="30"/>
       <c r="N5" s="31"/>
@@ -966,37 +1009,29 @@
       <c r="B6" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="22" t="n">
-        <v>40</v>
-      </c>
-      <c r="D6" s="23" t="n">
-        <v>90</v>
-      </c>
-      <c r="E6" s="24" t="n">
+      <c r="C6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="24" t="str">
         <f aca="false">IF(ISBLANK(D6),"no data",ABS($F$2-D6)/$F$2)</f>
-        <v>0.0526315789473684</v>
+        <v>no data</v>
       </c>
       <c r="F6" s="25" t="n">
         <f aca="false">IF(ISBLANK(D6),C6,IF(E6&gt;1,C6,C6+11*(1-E6)))</f>
-        <v>50.421052631579</v>
-      </c>
-      <c r="G6" s="26" t="n">
-        <v>60</v>
-      </c>
-      <c r="H6" s="27" t="n">
-        <v>190</v>
-      </c>
-      <c r="I6" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="26"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="24" t="str">
         <f aca="false">IF(ISBLANK(H6),"no data",ABS($J$2-H6)/$J$2)</f>
-        <v>0.177489177489178</v>
+        <v>no data</v>
       </c>
       <c r="J6" s="28" t="n">
         <f aca="false">IF(ISBLANK(H6),G6,IF(I6&gt;1,G6-17,G6+11*(1-I6)))</f>
-        <v>69.0476190476191</v>
+        <v>0</v>
       </c>
       <c r="K6" s="29" t="n">
         <f aca="false">AVERAGE(F6,J6)</f>
-        <v>59.734335839599</v>
+        <v>0</v>
       </c>
       <c r="L6" s="30" t="n">
         <f aca="false">RANK(K6, $K$5:$K$14)</f>
@@ -1038,7 +1073,7 @@
       </c>
       <c r="L7" s="30" t="n">
         <f aca="false">RANK(K7, $K$5:$K$14)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M7" s="34"/>
       <c r="N7" s="35"/>
@@ -1076,7 +1111,7 @@
       </c>
       <c r="L8" s="30" t="n">
         <f aca="false">RANK(K8, $K$5:$K$14)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M8" s="30"/>
       <c r="N8" s="31"/>
@@ -1114,7 +1149,7 @@
       </c>
       <c r="L9" s="30" t="n">
         <f aca="false">RANK(K9, $K$5:$K$14)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M9" s="30"/>
       <c r="N9" s="31"/>
@@ -1152,10 +1187,11 @@
       </c>
       <c r="L10" s="30" t="n">
         <f aca="false">RANK(K10, $K$5:$K$14)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M10" s="30"/>
       <c r="N10" s="31"/>
+      <c r="O10" s="37"/>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20" t="s">
@@ -1190,7 +1226,7 @@
       </c>
       <c r="L11" s="30" t="n">
         <f aca="false">RANK(K11, $K$5:$K$14)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M11" s="30"/>
       <c r="N11" s="31"/>
@@ -1228,7 +1264,7 @@
       </c>
       <c r="L12" s="30" t="n">
         <f aca="false">RANK(K12, $K$5:$K$14)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M12" s="30"/>
       <c r="N12" s="31"/>
@@ -1266,48 +1302,48 @@
       </c>
       <c r="L13" s="30" t="n">
         <f aca="false">RANK(K13, $K$5:$K$14)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M13" s="30"/>
       <c r="N13" s="31"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="24" t="str">
         <f aca="false">IF(ISBLANK(D14),"no data",ABS($F$2-D14)/$F$2)</f>
         <v>no data</v>
       </c>
-      <c r="F14" s="41" t="n">
+      <c r="F14" s="42" t="n">
         <f aca="false">IF(ISBLANK(D14),C14,IF(E14&gt;1,C14,C14+11*(1-E14)))</f>
         <v>0</v>
       </c>
-      <c r="G14" s="42"/>
-      <c r="H14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="44"/>
       <c r="I14" s="24" t="str">
         <f aca="false">IF(ISBLANK(H14),"no data",ABS($J$2-H14)/$J$2)</f>
         <v>no data</v>
       </c>
-      <c r="J14" s="44" t="n">
+      <c r="J14" s="45" t="n">
         <f aca="false">IF(ISBLANK(H14),G14,IF(I14&gt;1,G14-17,G14+11*(1-I14)))</f>
         <v>0</v>
       </c>
-      <c r="K14" s="45" t="n">
+      <c r="K14" s="46" t="n">
         <f aca="false">AVERAGE(F14,J14)</f>
         <v>0</v>
       </c>
-      <c r="L14" s="46" t="n">
+      <c r="L14" s="47" t="n">
         <f aca="false">RANK(K14, $K$5:$K$14)</f>
-        <v>3</v>
-      </c>
-      <c r="M14" s="46"/>
-      <c r="N14" s="47"/>
+        <v>1</v>
+      </c>
+      <c r="M14" s="47"/>
+      <c r="N14" s="48"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1316,7 +1352,6 @@
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C3:F3"/>

</xml_diff>